<commit_message>
🚸 Improve chart readability
</commit_message>
<xml_diff>
--- a/paperwork/paper/charts/pre_generated_charts/commit_percentage.xlsx
+++ b/paperwork/paper/charts/pre_generated_charts/commit_percentage.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ACEE1B0-E0BD-4937-B87A-AA6A30B8E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD19536B-53EC-4330-818A-326A09DAAB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Ilość zmian</t>
   </si>
@@ -42,16 +42,34 @@
     <t>Opis Zmiany</t>
   </si>
   <si>
-    <t>🔊</t>
+    <t>⚡️</t>
   </si>
   <si>
-    <t>Zarządzanie logami</t>
+    <t>Poprawki wydajności</t>
   </si>
   <si>
-    <t>🔥</t>
+    <t>🚚</t>
   </si>
   <si>
-    <t>Usuwanie martwego kodu</t>
+    <t>Przenoszenie zasobów/plików</t>
+  </si>
+  <si>
+    <t>🎨</t>
+  </si>
+  <si>
+    <t>Formatowanie kodu</t>
+  </si>
+  <si>
+    <t>📝</t>
+  </si>
+  <si>
+    <t>Pisanie dokumentacji</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>Dodawanie testów</t>
   </si>
   <si>
     <t>👷</t>
@@ -60,52 +78,22 @@
     <t>Rozwój systemu ciągłej integracji</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Inne</t>
+  </si>
+  <si>
     <t>🔨</t>
   </si>
   <si>
     <t>Rozwój narzędzi deweloperskich</t>
   </si>
   <si>
-    <t>♻️</t>
+    <t>✨</t>
   </si>
   <si>
-    <t>Refaktoryzacja kodu</t>
-  </si>
-  <si>
-    <t>🚚</t>
-  </si>
-  <si>
-    <t>Przenoszenie zasobów/plików</t>
-  </si>
-  <si>
-    <t>🚧</t>
-  </si>
-  <si>
-    <t>Prace tymczasowe</t>
-  </si>
-  <si>
-    <t>⚡️</t>
-  </si>
-  <si>
-    <t>Poprawki wydajności</t>
-  </si>
-  <si>
-    <t>✏️</t>
-  </si>
-  <si>
-    <t>Poprawki literówek</t>
-  </si>
-  <si>
-    <t>📝</t>
-  </si>
-  <si>
-    <t>Pisanie dokumentacji</t>
-  </si>
-  <si>
-    <t>💚</t>
-  </si>
-  <si>
-    <t>Naprawa systemu ciągłej integracji</t>
+    <t>Dodawanie nowych funkcjonalności</t>
   </si>
   <si>
     <t>🐛</t>
@@ -114,53 +102,17 @@
     <t>Naprawa błędów</t>
   </si>
   <si>
-    <t>🚨</t>
+    <t>♻️</t>
   </si>
   <si>
-    <t>Krytyczne naprawy</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Inne</t>
-  </si>
-  <si>
-    <t>🎨</t>
-  </si>
-  <si>
-    <t>Formatowanie kodu</t>
-  </si>
-  <si>
-    <t>✅</t>
-  </si>
-  <si>
-    <t>Dodawanie testów</t>
-  </si>
-  <si>
-    <t>✨</t>
-  </si>
-  <si>
-    <t>Dodawanie nowych funkcjonalności</t>
-  </si>
-  <si>
-    <t>➕</t>
-  </si>
-  <si>
-    <t>Aktualizacja zależności</t>
-  </si>
-  <si>
-    <t>🙈</t>
-  </si>
-  <si>
-    <t>Aktualizacja pliku .gitignore</t>
+    <t>Refaktoryzacja kodu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +125,13 @@
       <color theme="1"/>
       <name val="Liberation Sans"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,9 +154,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,6 +222,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -277,6 +242,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -292,6 +262,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -307,6 +282,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -322,6 +302,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -337,6 +322,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -354,6 +344,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -371,6 +366,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -388,6 +388,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -405,6 +410,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -422,6 +432,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -439,6 +454,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -457,6 +477,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -475,6 +500,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -493,6 +523,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -511,6 +546,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -529,6 +569,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -547,6 +592,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -564,6 +614,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -585,7 +640,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -629,125 +684,77 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$2:$B$20,Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$B$2:$B$12,Sheet1!$C$2:$C$12</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Zarządzanie logami</c:v>
+                    <c:v>Poprawki wydajności</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Usuwanie martwego kodu</c:v>
+                    <c:v>Przenoszenie zasobów/plików</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>Formatowanie kodu</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Pisanie dokumentacji</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dodawanie testów</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Rozwój systemu ciągłej integracji</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>Inne</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>Rozwój narzędzi deweloperskich</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>Dodawanie nowych funkcjonalności</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Naprawa błędów</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Refaktoryzacja kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Przenoszenie zasobów/plików</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Prace tymczasowe</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Poprawki wydajności</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Poprawki literówek</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Pisanie dokumentacji</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Naprawa systemu ciągłej integracji</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Naprawa błędów</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Krytyczne naprawy</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Inne</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Formatowanie kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Dodawanie testów</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Dodawanie nowych funkcjonalności</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Aktualizacja zależności</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Aktualizacja pliku .gitignore</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>🔊</c:v>
+                    <c:v>⚡️</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>🔥</c:v>
+                    <c:v>🚚</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>🎨</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>📝</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>✅</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>👷</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>?</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>🔨</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>✨</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>🐛</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>♻️</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>🚚</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>🚧</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>⚡️</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>✏️</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>📝</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>💚</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>🐛</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>🚨</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>?</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>🎨</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>✅</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>✨</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>➕</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>🙈</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -755,66 +762,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,6 +836,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -868,6 +856,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -883,6 +876,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -898,6 +896,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -913,6 +916,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -928,6 +936,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -945,6 +958,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -962,6 +980,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -979,6 +1002,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -996,6 +1024,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1013,6 +1046,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1030,6 +1068,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -1048,6 +1091,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -1066,6 +1114,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -1084,6 +1137,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -1102,6 +1160,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -1120,6 +1183,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -1138,6 +1206,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -1155,128 +1228,85 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$2:$B$20,Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$B$2:$B$12,Sheet1!$C$2:$C$12</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Zarządzanie logami</c:v>
+                    <c:v>Poprawki wydajności</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Usuwanie martwego kodu</c:v>
+                    <c:v>Przenoszenie zasobów/plików</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>Formatowanie kodu</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Pisanie dokumentacji</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dodawanie testów</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Rozwój systemu ciągłej integracji</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>Inne</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>Rozwój narzędzi deweloperskich</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>Dodawanie nowych funkcjonalności</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Naprawa błędów</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Refaktoryzacja kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Przenoszenie zasobów/plików</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Prace tymczasowe</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Poprawki wydajności</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Poprawki literówek</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Pisanie dokumentacji</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Naprawa systemu ciągłej integracji</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Naprawa błędów</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Krytyczne naprawy</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Inne</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Formatowanie kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Dodawanie testów</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Dodawanie nowych funkcjonalności</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Aktualizacja zależności</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Aktualizacja pliku .gitignore</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>🔊</c:v>
+                    <c:v>⚡️</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>🔥</c:v>
+                    <c:v>🚚</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>🎨</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>📝</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>✅</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>👷</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>?</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>🔨</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>✨</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>🐛</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>♻️</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>🚚</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>🚧</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>⚡️</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>✏️</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>📝</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>💚</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>🐛</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>🚨</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>?</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>🎨</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>✅</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>✨</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>➕</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>🙈</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1284,10 +1314,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1319,30 +1349,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1382,6 +1388,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1397,6 +1408,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1412,6 +1428,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1427,6 +1448,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1442,6 +1468,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1457,6 +1488,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1474,6 +1510,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1491,6 +1532,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1508,6 +1554,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1525,6 +1576,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1542,6 +1598,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1559,6 +1620,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -1577,6 +1643,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000065-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -1595,6 +1666,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000067-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -1613,6 +1689,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000069-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -1631,6 +1712,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006B-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -1649,6 +1735,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006D-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -1667,6 +1758,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006F-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -1684,128 +1780,85 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000071-6D4E-434A-B578-16F822FDE2BD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$2:$B$20,Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$B$2:$B$12,Sheet1!$C$2:$C$12</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Zarządzanie logami</c:v>
+                    <c:v>Poprawki wydajności</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Usuwanie martwego kodu</c:v>
+                    <c:v>Przenoszenie zasobów/plików</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>Formatowanie kodu</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Pisanie dokumentacji</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dodawanie testów</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Rozwój systemu ciągłej integracji</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>Inne</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>Rozwój narzędzi deweloperskich</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>Dodawanie nowych funkcjonalności</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Naprawa błędów</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>Refaktoryzacja kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Przenoszenie zasobów/plików</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Prace tymczasowe</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Poprawki wydajności</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Poprawki literówek</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Pisanie dokumentacji</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Naprawa systemu ciągłej integracji</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Naprawa błędów</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Krytyczne naprawy</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Inne</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Formatowanie kodu</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>Dodawanie testów</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Dodawanie nowych funkcjonalności</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>Aktualizacja zależności</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>Aktualizacja pliku .gitignore</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>🔊</c:v>
+                    <c:v>⚡️</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>🔥</c:v>
+                    <c:v>🚚</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>🎨</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>📝</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>✅</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>👷</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
+                    <c:v>?</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
                     <c:v>🔨</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="8">
+                    <c:v>✨</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>🐛</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>♻️</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>🚚</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>🚧</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>⚡️</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>✏️</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>📝</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>💚</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>🐛</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>🚨</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>?</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>🎨</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>✅</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>✨</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>➕</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>🙈</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1813,10 +1866,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1848,30 +1901,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2510,7 +2539,7 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2839,10 +2868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2865,7 +2894,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -2876,7 +2905,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -2887,7 +2916,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -2898,7 +2927,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -2909,7 +2938,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -2920,7 +2949,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -2931,7 +2960,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -2942,7 +2971,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -2953,7 +2982,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -2964,7 +2993,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -2975,7 +3004,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -2984,98 +3013,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>39</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>8</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>40</v>
-      </c>
+    <row r="19" spans="3:3">
+      <c r="C19" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C20" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
-      <sortCondition descending="1" ref="C1:C20"/>
+  <autoFilter ref="A1:C12" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
+      <sortCondition ref="A1:A12"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>